<commit_message>
cambie los colores al miercoles
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Edgardo\Docencia\Escuela 1 de 7\Excel\Ejercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Edgardo\Programación\Javascript\Clases\Concesionarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +73,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +101,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -340,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -351,6 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,7 +668,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,45 +677,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -716,7 +731,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="2">
         <v>4</v>
       </c>
@@ -740,7 +755,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="2">
         <v>11</v>
       </c>
@@ -764,7 +779,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2">
         <v>18</v>
       </c>
@@ -788,7 +803,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="4">
         <v>25</v>
       </c>

</xml_diff>